<commit_message>
update participants and oc
</commit_message>
<xml_diff>
--- a/hackthon/public/teams.xlsx
+++ b/hackthon/public/teams.xlsx
@@ -347,25 +347,25 @@
     <t>Naman Yadav</t>
   </si>
   <si>
-    <t>Cipher</t>
-  </si>
-  <si>
-    <t>HealthChain</t>
-  </si>
-  <si>
-    <t>IIMS College</t>
-  </si>
-  <si>
-    <t>Hemanta Acharya</t>
-  </si>
-  <si>
-    <t>Ishan Maharjan</t>
-  </si>
-  <si>
-    <t>Subit Timalsina</t>
-  </si>
-  <si>
-    <t>Smritee Kala Rai</t>
+    <t>Techtonic</t>
+  </si>
+  <si>
+    <t>Mind Bridge</t>
+  </si>
+  <si>
+    <t>IOE Purwanchal Campus</t>
+  </si>
+  <si>
+    <t>Jeevan Kumar Kushwaha</t>
+  </si>
+  <si>
+    <t>Kritam Bhattarai</t>
+  </si>
+  <si>
+    <t>Dipesh Acharya</t>
+  </si>
+  <si>
+    <t>Kushal Adhikari</t>
   </si>
   <si>
     <t>Yantra</t>
@@ -1159,13 +1159,13 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="16" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="35.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="47.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="16" width="30.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="42.57642857142857" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="16" width="11.862142857142858" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="16" width="19.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="16" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="16" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="16" width="18.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5" customFormat="1" s="1">

</xml_diff>

<commit_message>
project name update heignberg
</commit_message>
<xml_diff>
--- a/hackthon/public/teams.xlsx
+++ b/hackthon/public/teams.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="179">
   <si>
     <t>Team Name</t>
   </si>
@@ -416,6 +416,9 @@
     <t>Heisenberg</t>
   </si>
   <si>
+    <t>Automatic Accident Detection and Response System</t>
+  </si>
+  <si>
     <t>Adarsha Paudyal</t>
   </si>
   <si>
@@ -428,7 +431,7 @@
     <t>Tech Tacticos</t>
   </si>
   <si>
-    <t>Spinovate</t>
+    <t/>
   </si>
   <si>
     <t>Santosh Yadav</t>
@@ -784,7 +787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -820,6 +823,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -1164,14 +1170,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="16" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="30.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="42.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="16" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="16" width="19.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="16" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="16" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="30.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="42.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="17" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="17" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="17" width="18.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5" customFormat="1" s="1">
@@ -1200,7 +1206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -1278,7 +1284,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="10" t="s">
         <v>30</v>
       </c>
@@ -1304,7 +1310,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="6" t="s">
         <v>37</v>
       </c>
@@ -1671,19 +1677,19 @@
         <v>132</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>74</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>97</v>
@@ -1692,158 +1698,158 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="B21" s="11" t="s">
         <v>137</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>97</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
       <c r="A26" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
@@ -1937,14 +1943,14 @@
       <c r="H35" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="16.5">
-      <c r="A36" s="13"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
       <c r="G36" s="8"/>
-      <c r="H36" s="15"/>
+      <c r="H36" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>